<commit_message>
Actualización de Plan de Configuración
</commit_message>
<xml_diff>
--- a/Organizacional/Bisoltec-PlanConfiguracion.xlsx
+++ b/Organizacional/Bisoltec-PlanConfiguracion.xlsx
@@ -1,27 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="989"/>
   </bookViews>
   <sheets>
-    <sheet name="Proyectos" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Organizacional" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Proyectos" sheetId="1" r:id="rId1"/>
+    <sheet name="Organizacional" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" name="Complej." vbProcedure="false">#ref!</definedName>
-    <definedName function="false" hidden="false" name="Excel_BuiltIn_Print_Area_2" vbProcedure="false">#ref!</definedName>
-    <definedName function="false" hidden="false" name="Excel_BuiltIn_Print_Area_4" vbProcedure="false">#ref!</definedName>
+    <definedName name="Complej.">#REF!</definedName>
+    <definedName name="Excel_BuiltIn_Print_Area_2">#REF!</definedName>
+    <definedName name="Excel_BuiltIn_Print_Area_4">#REF!</definedName>
   </definedNames>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="134">
   <si>
     <t>Nombre de los Documentos</t>
   </si>
@@ -239,9 +238,6 @@
     <t>PTL-LevantamientoRequerimientos</t>
   </si>
   <si>
-    <t>Análisis de requerimientos</t>
-  </si>
-  <si>
     <t>PTL-AnalisisRequerimientos</t>
   </si>
   <si>
@@ -296,9 +292,6 @@
     <t>Bisoltec-AuditoriaOrganizacional-aammdd</t>
   </si>
   <si>
-    <t>Reporte conformidades</t>
-  </si>
-  <si>
     <t>Bisoltec-ReporteNoConformidades</t>
   </si>
   <si>
@@ -398,23 +391,44 @@
     <t>Cambios a los requerimientos</t>
   </si>
   <si>
+    <t>Reporte No Conformidades</t>
+  </si>
+  <si>
     <t>Respaldo</t>
   </si>
   <si>
     <t>Datos</t>
   </si>
   <si>
-    <t>Se genera un respaldo de la información de forma semestral ya que esta se encuentra en la nube, su almacenamiento debe estar registrado dentro de la carpeta Respaldos/respaldo_aammdd.zip</t>
+    <t>Herramienta</t>
+  </si>
+  <si>
+    <t>Responsable</t>
+  </si>
+  <si>
+    <t>Periodicidad</t>
+  </si>
+  <si>
+    <t>Jovanny Zepeda</t>
+  </si>
+  <si>
+    <t>Mensual</t>
+  </si>
+  <si>
+    <t>El respaldo estará ubicado dentro de la carpeta Respaldos/respaldo_aammdd.zip</t>
+  </si>
+  <si>
+    <t>Mecanismos para generación de la generación de la Línea Base</t>
+  </si>
+  <si>
+    <t>Seleccionar los archivos pertenecientes y agregarlos dentro de la carpeta Línea Base, que deberá estar dentro de la carpeta del proyecto. Agregar dichos archivos a repositorio, el responsable será el asignado en el Ciclo de Vida</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-  </numFmts>
-  <fonts count="13">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -422,22 +436,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="14"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial Narrow"/>
@@ -445,7 +444,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="12"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial Narrow"/>
@@ -485,7 +484,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="13"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial Narrow"/>
@@ -493,7 +492,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <u val="single"/>
+      <u/>
       <sz val="10"/>
       <color rgb="FF0563C1"/>
       <name val="Arial"/>
@@ -528,204 +527,147 @@
     </fill>
   </fills>
   <borders count="2">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="thin"/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="justify" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellXfs count="38">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="7">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -784,39 +726,47 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF404040"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>2311560</xdr:colOff>
+      <xdr:colOff>2284560</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>10440</xdr:rowOff>
+      <xdr:rowOff>19440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>207000</xdr:colOff>
+      <xdr:colOff>180360</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>834480</xdr:rowOff>
+      <xdr:rowOff>843840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="1 Imagen" descr=""/>
+        <xdr:cNvPr id="2" name="1 Imagen"/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId1"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7854840" y="10440"/>
-          <a:ext cx="2700720" cy="824040"/>
+          <a:off x="7827840" y="19440"/>
+          <a:ext cx="2701080" cy="824400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -832,33 +782,33 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>225360</xdr:colOff>
+      <xdr:colOff>198360</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>1080</xdr:rowOff>
+      <xdr:rowOff>10080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>425880</xdr:colOff>
+      <xdr:colOff>399240</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>825120</xdr:rowOff>
+      <xdr:rowOff>834480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1" name="1 Imagen" descr=""/>
+        <xdr:cNvPr id="2" name="1 Imagen"/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId1"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7614000" y="1080"/>
-          <a:ext cx="2620080" cy="824040"/>
+          <a:off x="7587000" y="10080"/>
+          <a:ext cx="2620440" cy="824400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -873,28 +823,308 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A14" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E28" activeCellId="0" sqref="E28"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="3.41836734693878"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="36.5714285714286"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="38.5714285714286"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="57.4234693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.6734693877551"/>
+    <col min="1" max="1" width="3.42578125"/>
+    <col min="2" max="2" width="36.5703125"/>
+    <col min="3" max="3" width="38.5703125"/>
+    <col min="4" max="4" width="57.42578125"/>
+    <col min="5" max="1025" width="10.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="67.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="3" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:4" ht="67.5" customHeight="1"/>
+    <row r="3" spans="1:4" ht="18">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -905,14 +1135,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:4" ht="18">
       <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="4"/>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:4" ht="15.75">
       <c r="A5" s="5"/>
       <c r="B5" s="6" t="s">
         <v>4</v>
@@ -920,7 +1150,7 @@
       <c r="C5" s="7"/>
       <c r="D5" s="8"/>
     </row>
-    <row r="6" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:4" ht="16.5">
       <c r="B6" s="9" t="s">
         <v>5</v>
       </c>
@@ -929,7 +1159,7 @@
       </c>
       <c r="D6" s="11"/>
     </row>
-    <row r="7" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:4" ht="16.5">
       <c r="B7" s="9" t="s">
         <v>7</v>
       </c>
@@ -940,7 +1170,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:4" ht="16.5">
       <c r="B8" s="9" t="s">
         <v>10</v>
       </c>
@@ -949,7 +1179,7 @@
       </c>
       <c r="D8" s="11"/>
     </row>
-    <row r="9" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:4" ht="16.5">
       <c r="A9" s="12"/>
       <c r="B9" s="9" t="s">
         <v>12</v>
@@ -961,7 +1191,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:4" ht="16.5">
       <c r="A10" s="12"/>
       <c r="B10" s="9" t="s">
         <v>14</v>
@@ -973,20 +1203,20 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:4" ht="16.5">
       <c r="A11" s="12"/>
       <c r="B11" s="13"/>
       <c r="C11" s="10"/>
       <c r="D11" s="11"/>
     </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:4" ht="15.75">
       <c r="B12" s="6" t="s">
         <v>16</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="8"/>
     </row>
-    <row r="13" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:4" ht="16.5">
       <c r="B13" s="9" t="s">
         <v>17</v>
       </c>
@@ -997,7 +1227,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:4" ht="16.5">
       <c r="B14" s="9" t="s">
         <v>19</v>
       </c>
@@ -1006,7 +1236,7 @@
       </c>
       <c r="D14" s="11"/>
     </row>
-    <row r="15" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:4" ht="16.5">
       <c r="B15" s="9" t="s">
         <v>21</v>
       </c>
@@ -1015,19 +1245,19 @@
       </c>
       <c r="D15" s="11"/>
     </row>
-    <row r="16" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:4" ht="16.5">
       <c r="B16" s="9"/>
       <c r="C16" s="10"/>
       <c r="D16" s="11"/>
     </row>
-    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:4" ht="15.75">
       <c r="B17" s="6" t="s">
         <v>23</v>
       </c>
       <c r="C17" s="7"/>
       <c r="D17" s="8"/>
     </row>
-    <row r="18" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:4" ht="16.5">
       <c r="B18" s="9" t="s">
         <v>24</v>
       </c>
@@ -1038,7 +1268,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:4" ht="16.5">
       <c r="B19" s="9" t="s">
         <v>26</v>
       </c>
@@ -1049,7 +1279,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:4" ht="16.5">
       <c r="B20" s="9" t="s">
         <v>28</v>
       </c>
@@ -1058,7 +1288,7 @@
       </c>
       <c r="D20" s="11"/>
     </row>
-    <row r="21" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:4" ht="16.5">
       <c r="B21" s="9" t="s">
         <v>30</v>
       </c>
@@ -1067,18 +1297,18 @@
       </c>
       <c r="D21" s="11"/>
     </row>
-    <row r="22" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:4" ht="16.5">
       <c r="C22" s="10"/>
       <c r="D22" s="11"/>
     </row>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:4" ht="15.75">
       <c r="B23" s="6" t="s">
         <v>32</v>
       </c>
       <c r="C23" s="7"/>
       <c r="D23" s="8"/>
     </row>
-    <row r="24" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:4" ht="18" customHeight="1">
       <c r="B24" s="14" t="s">
         <v>33</v>
       </c>
@@ -1089,9 +1319,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:4" ht="18" customHeight="1">
       <c r="A25" s="12"/>
-      <c r="B25" s="16" t="s">
+      <c r="B25" s="14" t="s">
         <v>35</v>
       </c>
       <c r="C25" s="15" t="s">
@@ -1099,14 +1329,14 @@
       </c>
       <c r="D25" s="16"/>
     </row>
-    <row r="26" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:4" ht="18" customHeight="1">
       <c r="B26" s="6" t="s">
         <v>37</v>
       </c>
       <c r="C26" s="7"/>
       <c r="D26" s="8"/>
     </row>
-    <row r="27" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:4" ht="18" customHeight="1">
       <c r="B27" s="14" t="s">
         <v>38</v>
       </c>
@@ -1115,7 +1345,7 @@
       </c>
       <c r="D27" s="11"/>
     </row>
-    <row r="28" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:4" ht="18" customHeight="1">
       <c r="B28" s="14" t="s">
         <v>40</v>
       </c>
@@ -1124,20 +1354,20 @@
       </c>
       <c r="D28" s="11"/>
     </row>
-    <row r="29" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:4" ht="16.5">
       <c r="A29" s="12"/>
       <c r="B29" s="17"/>
       <c r="C29" s="15"/>
       <c r="D29" s="11"/>
     </row>
-    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:4" ht="15.75">
       <c r="B30" s="6" t="s">
         <v>42</v>
       </c>
       <c r="C30" s="7"/>
       <c r="D30" s="8"/>
     </row>
-    <row r="31" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:4" ht="19.5" customHeight="1">
       <c r="B31" s="14" t="s">
         <v>43</v>
       </c>
@@ -1146,7 +1376,7 @@
       </c>
       <c r="D31" s="11"/>
     </row>
-    <row r="32" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:4" ht="19.5" customHeight="1">
       <c r="B32" s="14" t="s">
         <v>45</v>
       </c>
@@ -1155,18 +1385,18 @@
       </c>
       <c r="D32" s="11"/>
     </row>
-    <row r="33" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:4" ht="16.5">
       <c r="A33" s="12"/>
       <c r="D33" s="18"/>
     </row>
-    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:4" ht="15.75">
       <c r="B34" s="3" t="s">
         <v>47</v>
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="4"/>
     </row>
-    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:4" ht="15.75">
       <c r="A35" s="5"/>
       <c r="B35" s="19" t="s">
         <v>48</v>
@@ -1178,7 +1408,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="33.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:4" ht="33.75" customHeight="1">
       <c r="B36" s="21" t="s">
         <v>51</v>
       </c>
@@ -1189,7 +1419,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="37" spans="1:4" ht="18.75" customHeight="1">
       <c r="B37" s="21" t="s">
         <v>54</v>
       </c>
@@ -1200,7 +1430,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="38" spans="1:4" ht="18.75" customHeight="1">
       <c r="B38" s="21" t="s">
         <v>56</v>
       </c>
@@ -1211,7 +1441,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="39" spans="1:4" ht="18.75" customHeight="1">
       <c r="A39" s="12"/>
       <c r="B39" s="21" t="s">
         <v>59</v>
@@ -1223,44 +1453,70 @@
         <v>61</v>
       </c>
     </row>
+    <row r="41" spans="1:4" ht="16.5">
+      <c r="B41" s="36" t="s">
+        <v>132</v>
+      </c>
+      <c r="C41" s="36"/>
+      <c r="D41" s="23"/>
+    </row>
+    <row r="42" spans="1:4" ht="63.75" customHeight="1">
+      <c r="B42" s="37" t="s">
+        <v>133</v>
+      </c>
+      <c r="C42" s="37"/>
+      <c r="D42" s="23"/>
+    </row>
+    <row r="43" spans="1:4" ht="16.5">
+      <c r="B43" s="21"/>
+      <c r="C43" s="22"/>
+      <c r="D43" s="23"/>
+    </row>
+    <row r="44" spans="1:4" ht="16.5">
+      <c r="B44" s="21"/>
+      <c r="C44" s="22"/>
+      <c r="D44" s="11"/>
+    </row>
+    <row r="45" spans="1:4" ht="16.5">
+      <c r="B45" s="21"/>
+      <c r="C45" s="22"/>
+      <c r="D45" s="23"/>
+    </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <mergeCells count="2">
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:D52"/>
+  <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A35" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D52" activeCellId="0" sqref="D52"/>
+    <sheetView topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.86224489795918"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.8520408163265"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="64.0051020408163"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.2857142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.6734693877551"/>
+    <col min="1" max="1" width="4.85546875"/>
+    <col min="2" max="2" width="35.85546875"/>
+    <col min="3" max="3" width="56" customWidth="1"/>
+    <col min="4" max="4" width="34.28515625"/>
+    <col min="5" max="6" width="20.5703125" customWidth="1"/>
+    <col min="7" max="1025" width="10.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="67.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:4" ht="67.5" customHeight="1"/>
+    <row r="3" spans="1:4" ht="17.25" customHeight="1">
       <c r="B3" s="24"/>
       <c r="C3" s="24"/>
     </row>
-    <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:4" ht="17.25" customHeight="1">
       <c r="B4" s="25" t="s">
         <v>0</v>
       </c>
@@ -1268,7 +1524,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:4" ht="17.25" customHeight="1">
       <c r="B5" s="26" t="s">
         <v>62</v>
       </c>
@@ -1277,7 +1533,7 @@
       </c>
       <c r="D5" s="27"/>
     </row>
-    <row r="6" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:4" ht="17.25" customHeight="1">
       <c r="B6" s="26" t="s">
         <v>64</v>
       </c>
@@ -1286,7 +1542,7 @@
       </c>
       <c r="D6" s="27"/>
     </row>
-    <row r="7" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:4" ht="17.25" customHeight="1">
       <c r="B7" s="26" t="s">
         <v>66</v>
       </c>
@@ -1295,7 +1551,7 @@
       </c>
       <c r="D7" s="27"/>
     </row>
-    <row r="8" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:4" ht="17.25" customHeight="1">
       <c r="A8" s="12"/>
       <c r="B8" s="26" t="s">
         <v>68</v>
@@ -1305,14 +1561,14 @@
       </c>
       <c r="D8" s="27"/>
     </row>
-    <row r="9" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:4" ht="17.25" customHeight="1">
       <c r="B9" s="28" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="29"/>
       <c r="D9" s="27"/>
     </row>
-    <row r="10" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:4" ht="17.25" customHeight="1">
       <c r="B10" s="26" t="s">
         <v>70</v>
       </c>
@@ -1321,348 +1577,363 @@
       </c>
       <c r="D10" s="27"/>
     </row>
-    <row r="11" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:4" ht="17.25" customHeight="1">
       <c r="B11" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="C11" s="10" t="s">
-        <v>73</v>
-      </c>
       <c r="D11" s="27"/>
     </row>
-    <row r="12" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:4" ht="17.25" customHeight="1">
       <c r="B12" s="26" t="s">
         <v>10</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D12" s="27"/>
     </row>
-    <row r="13" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:4" ht="17.25" customHeight="1">
       <c r="B13" s="26" t="s">
         <v>12</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D13" s="27"/>
     </row>
-    <row r="14" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:4" ht="17.25" customHeight="1">
       <c r="A14" s="12"/>
       <c r="B14" s="26" t="s">
         <v>14</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D14" s="27"/>
     </row>
-    <row r="15" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:4" ht="17.25" customHeight="1">
       <c r="B15" s="28" t="s">
         <v>16</v>
       </c>
       <c r="C15" s="29"/>
       <c r="D15" s="27"/>
     </row>
-    <row r="16" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:4" ht="17.25" customHeight="1">
       <c r="B16" s="26" t="s">
         <v>17</v>
       </c>
       <c r="C16" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="D16" s="27"/>
+    </row>
+    <row r="17" spans="2:4" ht="17.25" customHeight="1">
+      <c r="B17" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="D16" s="27"/>
-    </row>
-    <row r="17" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B17" s="26" t="s">
+      <c r="C17" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="C17" s="10" t="s">
-        <v>79</v>
-      </c>
       <c r="D17" s="27"/>
     </row>
-    <row r="18" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="18" spans="2:4" ht="17.25" customHeight="1">
       <c r="B18" s="28" t="s">
         <v>23</v>
       </c>
       <c r="C18" s="29"/>
       <c r="D18" s="27"/>
     </row>
-    <row r="19" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="19" spans="2:4" ht="17.25" customHeight="1">
       <c r="B19" s="26" t="s">
         <v>28</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D19" s="27"/>
     </row>
-    <row r="20" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="20" spans="2:4" ht="17.25" customHeight="1">
       <c r="B20" s="28" t="s">
         <v>32</v>
       </c>
       <c r="C20" s="29"/>
       <c r="D20" s="27"/>
     </row>
-    <row r="21" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="21" spans="2:4" ht="17.25" customHeight="1">
       <c r="B21" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="C21" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="C21" s="15" t="s">
-        <v>82</v>
-      </c>
       <c r="D21" s="27"/>
     </row>
-    <row r="22" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="22" spans="2:4" ht="17.25" customHeight="1">
       <c r="B22" s="28" t="s">
         <v>37</v>
       </c>
       <c r="C22" s="29"/>
       <c r="D22" s="27"/>
     </row>
-    <row r="23" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="23" spans="2:4" ht="17.25" customHeight="1">
       <c r="B23" s="26" t="s">
         <v>38</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D23" s="27"/>
     </row>
-    <row r="24" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="24" spans="2:4" ht="17.25" customHeight="1">
       <c r="B24" s="26" t="s">
         <v>40</v>
       </c>
       <c r="C24" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="D24" s="27"/>
+    </row>
+    <row r="25" spans="2:4" ht="17.25" customHeight="1">
+      <c r="B25" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="D24" s="27"/>
-    </row>
-    <row r="25" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B25" s="26" t="s">
+      <c r="C25" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="C25" s="15" t="s">
+      <c r="D25" s="27"/>
+    </row>
+    <row r="26" spans="2:4" ht="17.25" customHeight="1">
+      <c r="B26" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="D25" s="27"/>
-    </row>
-    <row r="26" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B26" s="26" t="s">
+      <c r="C26" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="C26" s="15" t="s">
+      <c r="D26" s="27"/>
+    </row>
+    <row r="27" spans="2:4" ht="17.25" customHeight="1">
+      <c r="B27" s="28" t="s">
         <v>88</v>
-      </c>
-      <c r="D26" s="27"/>
-    </row>
-    <row r="27" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B27" s="28" t="s">
-        <v>89</v>
       </c>
       <c r="C27" s="29"/>
       <c r="D27" s="27"/>
     </row>
-    <row r="28" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="28" spans="2:4" ht="17.25" customHeight="1">
       <c r="B28" s="26" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C28" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="D28" s="27"/>
+    </row>
+    <row r="29" spans="2:4" ht="17.25" customHeight="1">
+      <c r="B29" s="26" t="s">
+        <v>123</v>
+      </c>
+      <c r="C29" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="D28" s="27"/>
-    </row>
-    <row r="29" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B29" s="26" t="s">
+      <c r="D29" s="27"/>
+    </row>
+    <row r="30" spans="2:4" ht="17.25" customHeight="1">
+      <c r="B30" s="28" t="s">
         <v>91</v>
-      </c>
-      <c r="C29" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="D29" s="27"/>
-    </row>
-    <row r="30" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B30" s="28" t="s">
-        <v>93</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="27"/>
     </row>
-    <row r="31" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="31" spans="2:4" ht="17.25" customHeight="1">
       <c r="B31" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="C31" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="D31" s="27"/>
+    </row>
+    <row r="32" spans="2:4" ht="17.25" customHeight="1">
+      <c r="B32" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="C31" s="15" t="s">
+      <c r="C32" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="D31" s="27"/>
-    </row>
-    <row r="32" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B32" s="26" t="s">
+      <c r="D32" s="27"/>
+    </row>
+    <row r="33" spans="1:4" ht="17.25" customHeight="1">
+      <c r="B33" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="C32" s="15" t="s">
+      <c r="C33" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="D32" s="27"/>
-    </row>
-    <row r="33" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B33" s="26" t="s">
+      <c r="D33" s="15"/>
+    </row>
+    <row r="34" spans="1:4" ht="17.25" customHeight="1">
+      <c r="B34" s="28" t="s">
         <v>98</v>
-      </c>
-      <c r="C33" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="D33" s="15"/>
-    </row>
-    <row r="34" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B34" s="28" t="s">
-        <v>100</v>
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="27"/>
     </row>
-    <row r="35" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:4" ht="17.25" customHeight="1">
       <c r="B35" s="26" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C35" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="D35" s="15"/>
+    </row>
+    <row r="36" spans="1:4" ht="17.25" customHeight="1">
+      <c r="B36" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="C36" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="D36" s="15"/>
+    </row>
+    <row r="37" spans="1:4" ht="17.25" customHeight="1">
+      <c r="B37" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="D35" s="15"/>
-    </row>
-    <row r="36" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B36" s="26" t="s">
-        <v>94</v>
-      </c>
-      <c r="C36" s="15" t="s">
+      <c r="C37" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="D36" s="15"/>
-    </row>
-    <row r="37" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B37" s="26" t="s">
+      <c r="D37" s="15"/>
+    </row>
+    <row r="38" spans="1:4" ht="17.25" customHeight="1">
+      <c r="B38" s="28" t="s">
         <v>103</v>
-      </c>
-      <c r="C37" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="D37" s="15"/>
-    </row>
-    <row r="38" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B38" s="28" t="s">
-        <v>105</v>
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="27"/>
     </row>
-    <row r="39" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="39" spans="1:4" ht="17.25" customHeight="1">
       <c r="B39" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="C39" s="15" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="17.25" customHeight="1">
+      <c r="B40" s="30" t="s">
         <v>106</v>
       </c>
-      <c r="C39" s="15" t="s">
+      <c r="C40" s="30" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="40" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B40" s="30" t="s">
+      <c r="D40" s="30" t="s">
         <v>108</v>
       </c>
-      <c r="C40" s="30" t="s">
+    </row>
+    <row r="41" spans="1:4" ht="17.25" customHeight="1">
+      <c r="B41" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="D40" s="30" t="s">
+      <c r="C41" s="31" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="41" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B41" s="18" t="s">
+      <c r="D41" s="32" t="s">
         <v>111</v>
       </c>
-      <c r="C41" s="31" t="s">
+    </row>
+    <row r="42" spans="1:4" ht="17.25" customHeight="1">
+      <c r="B42" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="D41" s="32" t="s">
+      <c r="C42" s="33" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="42" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B42" s="18" t="s">
+      <c r="D42" s="32" t="s">
         <v>114</v>
       </c>
-      <c r="C42" s="33" t="s">
-        <v>115</v>
-      </c>
-      <c r="D42" s="32" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="43" spans="1:4" ht="17.25" customHeight="1">
       <c r="A43" s="12"/>
       <c r="B43" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="C43" s="31" t="s">
+        <v>116</v>
+      </c>
+      <c r="D43" s="32" t="s">
         <v>117</v>
       </c>
-      <c r="C43" s="31" t="s">
+    </row>
+    <row r="44" spans="1:4" ht="17.25" customHeight="1">
+      <c r="B44" s="34"/>
+    </row>
+    <row r="45" spans="1:4" ht="17.25" customHeight="1">
+      <c r="B45" s="30" t="s">
         <v>118</v>
       </c>
-      <c r="D43" s="32" t="s">
+      <c r="C45" s="30" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="17.25" customHeight="1">
+      <c r="B46" s="18" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="44" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B44" s="34"/>
-    </row>
-    <row r="45" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B45" s="30" t="s">
+      <c r="C46" s="35" t="s">
         <v>120</v>
       </c>
-      <c r="C45" s="30" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B46" s="18" t="s">
+    </row>
+    <row r="47" spans="1:4" ht="17.25" customHeight="1">
+      <c r="B47" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="C46" s="35" t="s">
+      <c r="C47" s="35" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B47" s="18" t="s">
-        <v>123</v>
-      </c>
-      <c r="C47" s="35" t="s">
+    <row r="49" spans="2:6" ht="17.25">
+      <c r="B49" s="30" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="50" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B50" s="30" t="s">
+      <c r="C49" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="D49" s="30" t="s">
+        <v>126</v>
+      </c>
+      <c r="E49" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="F49" s="30" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" ht="33">
+      <c r="B50" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="C50" s="30" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="18" t="s">
-        <v>126</v>
-      </c>
-      <c r="C51" s="33" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="C50" s="35" t="s">
+        <v>131</v>
+      </c>
+      <c r="D50" s="35" t="s">
+        <v>112</v>
+      </c>
+      <c r="E50" s="35" t="s">
+        <v>129</v>
+      </c>
+      <c r="F50" s="35" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" ht="16.5">
+      <c r="B53" s="18"/>
+    </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>